<commit_message>
journal de travaille mis a jour +snénario ajouter
</commit_message>
<xml_diff>
--- a/Documents/Tableau de travail.xlsx
+++ b/Documents/Tableau de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\Bataille-Navale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6294AF-5EF5-495E-B8C3-C8046F02A8F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698D30F1-E86C-4AD9-9CE6-1E9DAFE97B69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -176,6 +176,33 @@
   </si>
   <si>
     <t>Colonne1</t>
+  </si>
+  <si>
+    <t>ecouter le prof</t>
+  </si>
+  <si>
+    <t>Le prof a parlé sur Les MCD</t>
+  </si>
+  <si>
+    <t>faire le MCD,Scénario,</t>
+  </si>
+  <si>
+    <t>j'ai commencé le MCD</t>
+  </si>
+  <si>
+    <t>j'ai continuer le MCD</t>
+  </si>
+  <si>
+    <t>j'ai continuer le MCD et commencer le Scénario</t>
+  </si>
+  <si>
+    <t>j'ai continuer le MCD et continuer le Scénario</t>
+  </si>
+  <si>
+    <t>j'ai fini le MCD et Le scénario</t>
+  </si>
+  <si>
+    <t>j'ai commencé le code de la bataille navale ,j'ai fait le menu</t>
   </si>
 </sst>
 </file>
@@ -727,7 +754,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,7 +767,7 @@
     <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -783,25 +810,42 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
-        <v>44244</v>
-      </c>
-      <c r="B2" s="7">
-        <v>0.5625</v>
-      </c>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="7">
-        <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>-0.5625</v>
-      </c>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="A3" s="6">
+        <v>44245</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="D3" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>38</v>
@@ -811,12 +855,36 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="6">
+        <v>44245</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.36458333333333331</v>
+      </c>
       <c r="D4" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>39</v>
@@ -826,12 +894,36 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="6">
+        <v>44245</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="D5" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>40</v>
@@ -842,37 +934,109 @@
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="6">
+        <v>44245</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.44097222222222227</v>
+      </c>
       <c r="D6" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="6">
+        <v>44245</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.47569444444444442</v>
+      </c>
       <c r="D7" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="6">
+        <v>44245</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D8" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
       </c>
       <c r="M8" s="18" t="s">
         <v>44</v>
       </c>
       <c r="N8" s="9">
         <f>COUNTIF(Tableau1[Terminé],"OUI")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -888,25 +1052,73 @@
       </c>
       <c r="N9" s="9">
         <f>COUNTIF(Tableau1[Terminé],"NON")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="6">
+        <v>44246</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.59375</v>
+      </c>
       <c r="D10" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="A11" s="6">
+        <v>44246</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D11" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1044,7 +1256,7 @@
       </c>
       <c r="N21" s="15">
         <f>SUMIF(Tableau1[Module],M21,Tableau1[Colonne1])</f>
-        <v>0</v>
+        <v>0.21874999999999994</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajout de la grille + essaie logs/scores
</commit_message>
<xml_diff>
--- a/Documents/Tableau de travail.xlsx
+++ b/Documents/Tableau de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\Bataille-Navale\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698D30F1-E86C-4AD9-9CE6-1E9DAFE97B69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580B5419-6D39-49BA-9C1D-F388E28CA01D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -203,6 +203,30 @@
   </si>
   <si>
     <t>j'ai commencé le code de la bataille navale ,j'ai fait le menu</t>
+  </si>
+  <si>
+    <t>continuer le code</t>
+  </si>
+  <si>
+    <t>j'ai continuer le code de la bataille navale, j'ai commencer le jeu</t>
+  </si>
+  <si>
+    <t>Le prof a parlé sur Les Maquettes</t>
+  </si>
+  <si>
+    <t>nous avons fait une maquette par groupe de quatre</t>
+  </si>
+  <si>
+    <t>faire une maquette HUD</t>
+  </si>
+  <si>
+    <t>presenter la maquette HUD</t>
+  </si>
+  <si>
+    <t>j'ai presenter HUD et ecouter les autres qui on presenter le leur</t>
+  </si>
+  <si>
+    <t>faire une maquette HUD 2.0</t>
   </si>
 </sst>
 </file>
@@ -754,7 +778,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,10 +788,10 @@
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -839,7 +863,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
         <v>48</v>
@@ -878,7 +902,7 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
         <v>50</v>
@@ -917,7 +941,7 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
         <v>51</v>
@@ -957,7 +981,7 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
         <v>52</v>
@@ -990,7 +1014,7 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
         <v>53</v>
@@ -1023,7 +1047,7 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
         <v>53</v>
@@ -1036,7 +1060,7 @@
       </c>
       <c r="N8" s="9">
         <f>COUNTIF(Tableau1[Terminé],"OUI")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1052,7 +1076,7 @@
       </c>
       <c r="N9" s="9">
         <f>COUNTIF(Tableau1[Terminé],"NON")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1131,21 +1155,69 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="A13" s="6">
+        <v>44258</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.59375</v>
+      </c>
       <c r="D13" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="A14" s="6">
+        <v>44258</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D14" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1164,28 +1236,76 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="6">
+        <v>44259</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.35069444444444442</v>
+      </c>
       <c r="D16" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>1.7361111111111105E-2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
       </c>
       <c r="M16" s="11" t="s">
         <v>19</v>
       </c>
       <c r="N16" s="14">
         <f>SUMIF(Tableau1[Module],M16,Tableau1[Colonne1])</f>
-        <v>0</v>
+        <v>0.26597222222222211</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="6">
+        <v>44259</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.36458333333333331</v>
+      </c>
       <c r="D17" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" t="s">
+        <v>16</v>
       </c>
       <c r="M17" s="12" t="s">
         <v>20</v>
@@ -1196,12 +1316,36 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="6">
+        <v>44259</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="D18" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
       </c>
       <c r="M18" s="12" t="s">
         <v>21</v>
@@ -1212,12 +1356,36 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="6">
+        <v>44259</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0.40625</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.44444444444444442</v>
+      </c>
       <c r="D19" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
       </c>
       <c r="M19" s="12" t="s">
         <v>22</v>
@@ -1228,12 +1396,30 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="6">
+        <v>44259</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.4458333333333333</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="D20" s="7">
         <f>Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[Heure de début]]</f>
-        <v>0</v>
+        <v>1.2500000000000011E-2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
       </c>
       <c r="M20" s="12" t="s">
         <v>23</v>
@@ -1256,7 +1442,7 @@
       </c>
       <c r="N21" s="15">
         <f>SUMIF(Tableau1[Module],M21,Tableau1[Colonne1])</f>
-        <v>0.21874999999999994</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>